<commit_message>
adicionado novos requisitos em agendamento
</commit_message>
<xml_diff>
--- a/artefatos/Requisitos de Sistemas.xlsx
+++ b/artefatos/Requisitos de Sistemas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>SSS0001</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>SSS0019</t>
+  </si>
+  <si>
+    <t>O sistema DEVE permitir que o cliente veja quanto foi o valor total de seu agendamento</t>
+  </si>
+  <si>
+    <t>SSS0020</t>
+  </si>
+  <si>
+    <t>O sistema DEVE permitir que o cliente altere o procedimento de seu agendamento</t>
+  </si>
+  <si>
+    <t>SSS0021</t>
   </si>
 </sst>
 </file>
@@ -145,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,8 +182,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -233,58 +251,109 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,16 +656,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I38"/>
+  <dimension ref="A2:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -608,45 +677,45 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -654,12 +723,12 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -668,7 +737,7 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -676,188 +745,188 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -866,7 +935,7 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -875,33 +944,33 @@
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="B27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -910,7 +979,7 @@
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -919,132 +988,180 @@
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="14" t="s">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="14" t="s">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="16"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="14" t="s">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="B31:G32"/>
-    <mergeCell ref="B33:G34"/>
-    <mergeCell ref="B35:G36"/>
-    <mergeCell ref="B37:G38"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
+  <mergeCells count="41">
+    <mergeCell ref="B3:G4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B11:G12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B5:G6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B7:G8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B15:G16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B19:G20"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B13:G14"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="B21:G22"/>
     <mergeCell ref="B23:G24"/>
-    <mergeCell ref="B25:G26"/>
-    <mergeCell ref="B27:G28"/>
-    <mergeCell ref="B29:G30"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B19:G20"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B11:G12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B13:G14"/>
-    <mergeCell ref="B15:G16"/>
-    <mergeCell ref="B7:G8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B9:G10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5:G6"/>
-    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B25:G26"/>
+    <mergeCell ref="B27:G28"/>
+    <mergeCell ref="B29:G30"/>
+    <mergeCell ref="B31:G32"/>
+    <mergeCell ref="B33:G34"/>
+    <mergeCell ref="B35:G36"/>
+    <mergeCell ref="B37:G38"/>
+    <mergeCell ref="B39:G40"/>
+    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>